<commit_message>
fixed variable names and rebuilt emx
</commit_message>
<xml_diff>
--- a/emx/cosas-portal/cosasportal.xlsx
+++ b/emx/cosas-portal/cosasportal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">COSAS Portal</t>
   </si>
   <si>
-    <t xml:space="preserve">Staging tables for raw data extracts (v0.901, 2021-08-19)</t>
+    <t xml:space="preserve">Staging tables for raw data extracts (v0.9011, 2021-08-30)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t xml:space="preserve">created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenotype</t>
   </si>
 </sst>
 </file>
@@ -4171,13 +4174,13 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="B128" t="s">
         <v>144</v>
       </c>
       <c r="C128" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D128"/>
       <c r="E128"/>
@@ -4195,31 +4198,55 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B129" t="s">
         <v>144</v>
       </c>
       <c r="C129" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D129"/>
-      <c r="E129" t="s">
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="G129" t="b">
+        <v>0</v>
+      </c>
+      <c r="H129"/>
+      <c r="I129" t="b">
+        <v>1</v>
+      </c>
+      <c r="J129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>64</v>
+      </c>
+      <c r="B130" t="s">
+        <v>144</v>
+      </c>
+      <c r="C130" t="s">
+        <v>51</v>
+      </c>
+      <c r="D130"/>
+      <c r="E130" t="s">
         <v>65</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F130" t="s">
         <v>66</v>
       </c>
-      <c r="G129" t="b">
-        <v>1</v>
-      </c>
-      <c r="H129" t="b">
-        <v>1</v>
-      </c>
-      <c r="I129" t="b">
-        <v>0</v>
-      </c>
-      <c r="J129" t="b">
+      <c r="G130" t="b">
+        <v>1</v>
+      </c>
+      <c r="H130" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130" t="b">
+        <v>0</v>
+      </c>
+      <c r="J130" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>